<commit_message>
Week 8 documentations added
</commit_message>
<xml_diff>
--- a/documents/G05_Week8/项目周报_G05_B_w08.xlsx
+++ b/documents/G05_Week8/项目周报_G05_B_w08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\my751\IdeaProjects\PetHospital\documents\G05_Week8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F787FFD8-9A08-4D59-A621-0BF509B24404}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBD2651-2A82-497C-87D0-8903EE38889E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E1701B8E-C766-4E73-A45B-EFE082D1FEF4}"/>
   </bookViews>
@@ -51,10 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2021/4/1-2020/4/7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>系统开发，接口测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -64,6 +60,10 @@
   </si>
   <si>
     <t>组织相关前端开发人员进行集中技术攻关，阅读相关技术文档，集中开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021/4/14-2020/4/21</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -479,7 +479,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -501,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="42.6" customHeight="1" x14ac:dyDescent="0.4">
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.4">
@@ -525,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="54.6" customHeight="1" x14ac:dyDescent="0.4">
@@ -533,7 +533,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>